<commit_message>
Done with the Exceptions for the Excel File Upload.
Need to update the swal for a nice view of the exception.
</commit_message>
<xml_diff>
--- a/KinartiProject_ruppin/uploadedFiles/work_flow.xlsx
+++ b/KinartiProject_ruppin/uploadedFiles/work_flow.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\test\work flow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.tochilovsky\Desktop\Certs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -145,9 +145,6 @@
     <t>כמות</t>
   </si>
   <si>
-    <t>אלכס</t>
-  </si>
-  <si>
     <t>P001</t>
   </si>
   <si>
@@ -163,9 +160,6 @@
     <t>Liv_3111_1</t>
   </si>
   <si>
-    <t>1414P001</t>
-  </si>
-  <si>
     <t>מסור גשר</t>
   </si>
   <si>
@@ -184,27 +178,18 @@
     <t xml:space="preserve">Liv_3111_2 </t>
   </si>
   <si>
-    <t>1414P002</t>
-  </si>
-  <si>
     <t>P003</t>
   </si>
   <si>
     <t>P003-1</t>
   </si>
   <si>
-    <t>1414P003</t>
-  </si>
-  <si>
     <t>P004</t>
   </si>
   <si>
     <t>P004-1</t>
   </si>
   <si>
-    <t>1414P004</t>
-  </si>
-  <si>
     <t>P005</t>
   </si>
   <si>
@@ -217,9 +202,6 @@
     <t>P005-1</t>
   </si>
   <si>
-    <t>1414P005</t>
-  </si>
-  <si>
     <t>נסטיג</t>
   </si>
   <si>
@@ -232,9 +214,6 @@
     <t>P006-1</t>
   </si>
   <si>
-    <t>1414P006</t>
-  </si>
-  <si>
     <t>P007</t>
   </si>
   <si>
@@ -244,27 +223,18 @@
     <t>P007-1</t>
   </si>
   <si>
-    <t>1414P007</t>
-  </si>
-  <si>
     <t>P008</t>
   </si>
   <si>
     <t>P008-1</t>
   </si>
   <si>
-    <t>1414P008</t>
-  </si>
-  <si>
     <t>P009</t>
   </si>
   <si>
     <t>P009-1</t>
   </si>
   <si>
-    <t>1414P009</t>
-  </si>
-  <si>
     <t>P010</t>
   </si>
   <si>
@@ -280,27 +250,18 @@
     <t>QE 4003 טמבור</t>
   </si>
   <si>
-    <t>1414P010</t>
-  </si>
-  <si>
     <t>P011</t>
   </si>
   <si>
     <t>P011-1</t>
   </si>
   <si>
-    <t>1414P011</t>
-  </si>
-  <si>
     <t>P012</t>
   </si>
   <si>
     <t>P012-1</t>
   </si>
   <si>
-    <t>1414P012</t>
-  </si>
-  <si>
     <t>P013</t>
   </si>
   <si>
@@ -310,9 +271,6 @@
     <t>P013-1</t>
   </si>
   <si>
-    <t>1414P013</t>
-  </si>
-  <si>
     <t>P014</t>
   </si>
   <si>
@@ -322,27 +280,18 @@
     <t>P014-1</t>
   </si>
   <si>
-    <t>1414P014</t>
-  </si>
-  <si>
     <t>P015</t>
   </si>
   <si>
     <t>P015-1</t>
   </si>
   <si>
-    <t>1414P015</t>
-  </si>
-  <si>
     <t>P016</t>
   </si>
   <si>
     <t>P016-1</t>
   </si>
   <si>
-    <t>1414P016</t>
-  </si>
-  <si>
     <t>P017</t>
   </si>
   <si>
@@ -355,27 +304,18 @@
     <t>P017-1</t>
   </si>
   <si>
-    <t>1414P017</t>
-  </si>
-  <si>
     <t>P018</t>
   </si>
   <si>
     <t>P018-1</t>
   </si>
   <si>
-    <t>1414P018</t>
-  </si>
-  <si>
     <t>P019</t>
   </si>
   <si>
     <t>P019-1</t>
   </si>
   <si>
-    <t>1414P019</t>
-  </si>
-  <si>
     <t>P020</t>
   </si>
   <si>
@@ -385,9 +325,6 @@
     <t>P020-1</t>
   </si>
   <si>
-    <t>1414P020</t>
-  </si>
-  <si>
     <t>P021</t>
   </si>
   <si>
@@ -397,27 +334,18 @@
     <t>P021-1</t>
   </si>
   <si>
-    <t>1414P021</t>
-  </si>
-  <si>
     <t>P022</t>
   </si>
   <si>
     <t>P022-1</t>
   </si>
   <si>
-    <t>1414P022</t>
-  </si>
-  <si>
     <t>P023</t>
   </si>
   <si>
     <t>P023-1</t>
   </si>
   <si>
-    <t>1414P023</t>
-  </si>
-  <si>
     <t>P024</t>
   </si>
   <si>
@@ -427,9 +355,6 @@
     <t>Liv_Alon_1</t>
   </si>
   <si>
-    <t>1414P024</t>
-  </si>
-  <si>
     <t>להדביק גריל אויר</t>
   </si>
   <si>
@@ -442,18 +367,12 @@
     <t>P025-1</t>
   </si>
   <si>
-    <t>1414P025</t>
-  </si>
-  <si>
     <t>P026</t>
   </si>
   <si>
     <t>P026-1</t>
   </si>
   <si>
-    <t>1414P026</t>
-  </si>
-  <si>
     <t>P027</t>
   </si>
   <si>
@@ -469,9 +388,6 @@
     <t>פורניר אגוז אנכי</t>
   </si>
   <si>
-    <t>1414P027</t>
-  </si>
-  <si>
     <t>חלקים להדבקת פורניר</t>
   </si>
   <si>
@@ -484,9 +400,6 @@
     <t>P028-1</t>
   </si>
   <si>
-    <t>1414P028</t>
-  </si>
-  <si>
     <t>P029</t>
   </si>
   <si>
@@ -496,9 +409,6 @@
     <t>P029-1</t>
   </si>
   <si>
-    <t>1414P029</t>
-  </si>
-  <si>
     <t>P030</t>
   </si>
   <si>
@@ -508,9 +418,6 @@
     <t>P030-1</t>
   </si>
   <si>
-    <t>1414P030</t>
-  </si>
-  <si>
     <t>חלקים לעבודת נגר</t>
   </si>
   <si>
@@ -523,9 +430,6 @@
     <t>P031-1</t>
   </si>
   <si>
-    <t>1414P031</t>
-  </si>
-  <si>
     <t>P032</t>
   </si>
   <si>
@@ -535,13 +439,109 @@
     <t>P032-2</t>
   </si>
   <si>
-    <t>1414P032</t>
+    <t>עינב</t>
+  </si>
+  <si>
+    <t>1212P001</t>
+  </si>
+  <si>
+    <t>1212P002</t>
+  </si>
+  <si>
+    <t>1212P003</t>
+  </si>
+  <si>
+    <t>1212P004</t>
+  </si>
+  <si>
+    <t>1212P005</t>
+  </si>
+  <si>
+    <t>1212P006</t>
+  </si>
+  <si>
+    <t>1212P007</t>
+  </si>
+  <si>
+    <t>1212P008</t>
+  </si>
+  <si>
+    <t>1212P009</t>
+  </si>
+  <si>
+    <t>1212P010</t>
+  </si>
+  <si>
+    <t>1212P011</t>
+  </si>
+  <si>
+    <t>1212P012</t>
+  </si>
+  <si>
+    <t>1212P013</t>
+  </si>
+  <si>
+    <t>1212P014</t>
+  </si>
+  <si>
+    <t>1212P015</t>
+  </si>
+  <si>
+    <t>1212P016</t>
+  </si>
+  <si>
+    <t>1212P017</t>
+  </si>
+  <si>
+    <t>1212P018</t>
+  </si>
+  <si>
+    <t>1212P019</t>
+  </si>
+  <si>
+    <t>1212P020</t>
+  </si>
+  <si>
+    <t>1212P021</t>
+  </si>
+  <si>
+    <t>1212P022</t>
+  </si>
+  <si>
+    <t>1212P023</t>
+  </si>
+  <si>
+    <t>1212P024</t>
+  </si>
+  <si>
+    <t>1212P025</t>
+  </si>
+  <si>
+    <t>1212P026</t>
+  </si>
+  <si>
+    <t>1212P027</t>
+  </si>
+  <si>
+    <t>1212P028</t>
+  </si>
+  <si>
+    <t>1212P029</t>
+  </si>
+  <si>
+    <t>1212P030</t>
+  </si>
+  <si>
+    <t>1212P031</t>
+  </si>
+  <si>
+    <t>1212P032</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -599,7 +599,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -864,12 +864,14 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="18.85546875" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
@@ -945,31 +947,31 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2">
+        <v>1122</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>23</v>
       </c>
-      <c r="C2">
-        <v>1414</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>27</v>
-      </c>
-      <c r="J2" t="s">
-        <v>28</v>
       </c>
       <c r="L2">
         <v>959</v>
@@ -990,13 +992,13 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>29</v>
+        <v>122</v>
       </c>
       <c r="S2" t="s">
-        <v>29</v>
+        <v>122</v>
       </c>
       <c r="T2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W2">
         <v>1</v>
@@ -1004,31 +1006,31 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C3">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
         <v>31</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>32</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>33</v>
-      </c>
-      <c r="H3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" t="s">
-        <v>35</v>
       </c>
       <c r="L3">
         <v>624</v>
@@ -1049,13 +1051,13 @@
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>36</v>
+        <v>123</v>
       </c>
       <c r="S3" t="s">
-        <v>36</v>
+        <v>123</v>
       </c>
       <c r="T3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W3">
         <v>1</v>
@@ -1063,31 +1065,31 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C4">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" t="s">
         <v>33</v>
-      </c>
-      <c r="H4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" t="s">
-        <v>35</v>
       </c>
       <c r="L4">
         <v>624</v>
@@ -1108,13 +1110,13 @@
         <v>0</v>
       </c>
       <c r="R4" t="s">
-        <v>39</v>
+        <v>124</v>
       </c>
       <c r="S4" t="s">
-        <v>39</v>
+        <v>124</v>
       </c>
       <c r="T4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W4">
         <v>1</v>
@@ -1122,31 +1124,31 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C5">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" t="s">
         <v>33</v>
-      </c>
-      <c r="H5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" t="s">
-        <v>35</v>
       </c>
       <c r="L5">
         <v>624</v>
@@ -1167,13 +1169,13 @@
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
       <c r="S5" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
       <c r="T5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W5">
         <v>1</v>
@@ -1181,31 +1183,31 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C6">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L6">
         <v>960</v>
@@ -1226,13 +1228,13 @@
         <v>0</v>
       </c>
       <c r="R6" t="s">
-        <v>47</v>
+        <v>126</v>
       </c>
       <c r="S6" t="s">
-        <v>47</v>
+        <v>126</v>
       </c>
       <c r="T6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="W6">
         <v>1</v>
@@ -1240,31 +1242,31 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C7">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" t="s">
         <v>45</v>
       </c>
-      <c r="H7" t="s">
-        <v>51</v>
-      </c>
       <c r="J7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L7">
         <v>960</v>
@@ -1285,13 +1287,13 @@
         <v>0</v>
       </c>
       <c r="R7" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="S7" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="T7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="W7">
         <v>1</v>
@@ -1299,31 +1301,31 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C8">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" t="s">
         <v>33</v>
-      </c>
-      <c r="H8" t="s">
-        <v>55</v>
-      </c>
-      <c r="J8" t="s">
-        <v>35</v>
       </c>
       <c r="L8">
         <v>624</v>
@@ -1344,13 +1346,13 @@
         <v>0</v>
       </c>
       <c r="R8" t="s">
-        <v>56</v>
+        <v>128</v>
       </c>
       <c r="S8" t="s">
-        <v>56</v>
+        <v>128</v>
       </c>
       <c r="T8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W8">
         <v>1</v>
@@ -1358,31 +1360,31 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C9">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" t="s">
         <v>33</v>
-      </c>
-      <c r="H9" t="s">
-        <v>58</v>
-      </c>
-      <c r="J9" t="s">
-        <v>35</v>
       </c>
       <c r="L9">
         <v>624</v>
@@ -1403,13 +1405,13 @@
         <v>0</v>
       </c>
       <c r="R9" t="s">
-        <v>59</v>
+        <v>129</v>
       </c>
       <c r="S9" t="s">
-        <v>59</v>
+        <v>129</v>
       </c>
       <c r="T9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W9">
         <v>1</v>
@@ -1417,31 +1419,31 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C10">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" t="s">
         <v>33</v>
-      </c>
-      <c r="H10" t="s">
-        <v>61</v>
-      </c>
-      <c r="J10" t="s">
-        <v>35</v>
       </c>
       <c r="L10">
         <v>624</v>
@@ -1462,13 +1464,13 @@
         <v>0</v>
       </c>
       <c r="R10" t="s">
-        <v>62</v>
+        <v>130</v>
       </c>
       <c r="S10" t="s">
-        <v>62</v>
+        <v>130</v>
       </c>
       <c r="T10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W10">
         <v>1</v>
@@ -1476,34 +1478,34 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C11">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F11" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="J11" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="K11" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="L11">
         <v>700</v>
@@ -1524,13 +1526,13 @@
         <v>0</v>
       </c>
       <c r="R11" t="s">
-        <v>68</v>
+        <v>131</v>
       </c>
       <c r="S11" t="s">
-        <v>68</v>
+        <v>131</v>
       </c>
       <c r="T11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="W11">
         <v>1</v>
@@ -1538,34 +1540,34 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C12">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="F12" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H12" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="J12" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="K12" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="L12">
         <v>700</v>
@@ -1586,13 +1588,13 @@
         <v>0</v>
       </c>
       <c r="R12" t="s">
-        <v>71</v>
+        <v>132</v>
       </c>
       <c r="S12" t="s">
-        <v>71</v>
+        <v>132</v>
       </c>
       <c r="T12" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="W12">
         <v>1</v>
@@ -1600,34 +1602,34 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C13">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="F13" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H13" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="J13" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="K13" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="L13">
         <v>700</v>
@@ -1648,13 +1650,13 @@
         <v>0</v>
       </c>
       <c r="R13" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="S13" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="T13" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="W13">
         <v>1</v>
@@ -1662,31 +1664,31 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C14">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H14" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="J14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L14">
         <v>666</v>
@@ -1707,13 +1709,13 @@
         <v>0</v>
       </c>
       <c r="R14" t="s">
-        <v>78</v>
+        <v>134</v>
       </c>
       <c r="S14" t="s">
-        <v>78</v>
+        <v>134</v>
       </c>
       <c r="T14" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="W14">
         <v>1</v>
@@ -1721,31 +1723,31 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C15">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="F15" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="G15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" t="s">
         <v>33</v>
-      </c>
-      <c r="H15" t="s">
-        <v>81</v>
-      </c>
-      <c r="J15" t="s">
-        <v>35</v>
       </c>
       <c r="L15">
         <v>440</v>
@@ -1766,13 +1768,13 @@
         <v>0</v>
       </c>
       <c r="R15" t="s">
-        <v>82</v>
+        <v>135</v>
       </c>
       <c r="S15" t="s">
-        <v>82</v>
+        <v>135</v>
       </c>
       <c r="T15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W15">
         <v>1</v>
@@ -1780,31 +1782,31 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C16">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="F16" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="G16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" t="s">
+        <v>69</v>
+      </c>
+      <c r="J16" t="s">
         <v>33</v>
-      </c>
-      <c r="H16" t="s">
-        <v>84</v>
-      </c>
-      <c r="J16" t="s">
-        <v>35</v>
       </c>
       <c r="L16">
         <v>440</v>
@@ -1825,13 +1827,13 @@
         <v>0</v>
       </c>
       <c r="R16" t="s">
-        <v>85</v>
+        <v>136</v>
       </c>
       <c r="S16" t="s">
-        <v>85</v>
+        <v>136</v>
       </c>
       <c r="T16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W16">
         <v>1</v>
@@ -1839,31 +1841,31 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C17">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="G17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" t="s">
+        <v>71</v>
+      </c>
+      <c r="J17" t="s">
         <v>33</v>
-      </c>
-      <c r="H17" t="s">
-        <v>87</v>
-      </c>
-      <c r="J17" t="s">
-        <v>35</v>
       </c>
       <c r="L17">
         <v>440</v>
@@ -1884,13 +1886,13 @@
         <v>0</v>
       </c>
       <c r="R17" t="s">
-        <v>88</v>
+        <v>137</v>
       </c>
       <c r="S17" t="s">
-        <v>88</v>
+        <v>137</v>
       </c>
       <c r="T17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W17">
         <v>1</v>
@@ -1898,31 +1900,31 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C18">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="F18" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="G18" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="H18" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="J18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L18">
         <v>440</v>
@@ -1943,13 +1945,13 @@
         <v>0</v>
       </c>
       <c r="R18" t="s">
-        <v>93</v>
+        <v>138</v>
       </c>
       <c r="S18" t="s">
-        <v>93</v>
+        <v>138</v>
       </c>
       <c r="T18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W18">
         <v>1</v>
@@ -1957,31 +1959,31 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C19">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="F19" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="G19" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="H19" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="J19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L19">
         <v>440</v>
@@ -2002,13 +2004,13 @@
         <v>0</v>
       </c>
       <c r="R19" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
       <c r="S19" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
       <c r="T19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W19">
         <v>1</v>
@@ -2016,31 +2018,31 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C20">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="F20" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="G20" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="H20" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="J20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L20">
         <v>440</v>
@@ -2061,13 +2063,13 @@
         <v>0</v>
       </c>
       <c r="R20" t="s">
-        <v>99</v>
+        <v>140</v>
       </c>
       <c r="S20" t="s">
-        <v>99</v>
+        <v>140</v>
       </c>
       <c r="T20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W20">
         <v>1</v>
@@ -2075,31 +2077,31 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C21">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F21" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="G21" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H21" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="J21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L21">
         <v>666</v>
@@ -2120,13 +2122,13 @@
         <v>0</v>
       </c>
       <c r="R21" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="S21" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="T21" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="W21">
         <v>1</v>
@@ -2134,31 +2136,31 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C22">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="F22" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="G22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H22" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="J22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L22">
         <v>636</v>
@@ -2179,13 +2181,13 @@
         <v>0</v>
       </c>
       <c r="R22" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="S22" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="T22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W22">
         <v>1</v>
@@ -2193,31 +2195,31 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C23">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="F23" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="G23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H23" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="J23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L23">
         <v>636</v>
@@ -2238,13 +2240,13 @@
         <v>0</v>
       </c>
       <c r="R23" t="s">
-        <v>110</v>
+        <v>143</v>
       </c>
       <c r="S23" t="s">
-        <v>110</v>
+        <v>143</v>
       </c>
       <c r="T23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W23">
         <v>1</v>
@@ -2252,31 +2254,31 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C24">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="F24" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="G24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H24" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="J24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L24">
         <v>636</v>
@@ -2297,13 +2299,13 @@
         <v>0</v>
       </c>
       <c r="R24" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="S24" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="T24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W24">
         <v>1</v>
@@ -2311,31 +2313,31 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C25">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="F25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" t="s">
         <v>25</v>
       </c>
-      <c r="G25" t="s">
-        <v>26</v>
-      </c>
       <c r="H25" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="J25" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="L25">
         <v>814</v>
@@ -2356,16 +2358,16 @@
         <v>0</v>
       </c>
       <c r="R25" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="S25" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="T25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V25" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="W25">
         <v>1</v>
@@ -2373,31 +2375,31 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C26">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="F26" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G26" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="H26" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="J26" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="L26">
         <v>815</v>
@@ -2418,13 +2420,13 @@
         <v>0</v>
       </c>
       <c r="R26" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="S26" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="T26" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="W26">
         <v>1</v>
@@ -2432,31 +2434,31 @@
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C27">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="F27" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G27" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="H27" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="J27" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="L27">
         <v>815</v>
@@ -2477,13 +2479,13 @@
         <v>0</v>
       </c>
       <c r="R27" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="S27" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="T27" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="W27">
         <v>1</v>
@@ -2491,34 +2493,34 @@
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C28">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="F28" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="G28" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
       <c r="H28" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="J28" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="K28" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="L28">
         <v>814</v>
@@ -2539,16 +2541,16 @@
         <v>0</v>
       </c>
       <c r="R28" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="S28" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="T28" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="U28" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="W28">
         <v>1</v>
@@ -2556,34 +2558,34 @@
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C29">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="F29" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="G29" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
       <c r="H29" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="J29" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="K29" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="L29">
         <v>814</v>
@@ -2604,16 +2606,16 @@
         <v>0</v>
       </c>
       <c r="R29" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="S29" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="T29" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="U29" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="W29">
         <v>1</v>
@@ -2621,31 +2623,31 @@
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C30">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D30">
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="F30" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
       <c r="G30" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="H30" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="J30" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="L30">
         <v>566</v>
@@ -2666,13 +2668,13 @@
         <v>0</v>
       </c>
       <c r="R30" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="S30" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="T30" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="W30">
         <v>1</v>
@@ -2680,31 +2682,31 @@
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C31">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
       <c r="F31" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
       <c r="G31" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="H31" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="J31" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="L31">
         <v>566</v>
@@ -2725,16 +2727,16 @@
         <v>0</v>
       </c>
       <c r="R31" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="S31" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="T31" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="U31" t="s">
-        <v>145</v>
+        <v>114</v>
       </c>
       <c r="W31">
         <v>1</v>
@@ -2742,31 +2744,31 @@
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C32">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D32">
         <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
       <c r="F32" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="G32" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="H32" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
       <c r="J32" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="L32">
         <v>566</v>
@@ -2787,16 +2789,16 @@
         <v>0</v>
       </c>
       <c r="R32" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="S32" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="T32" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="U32" t="s">
-        <v>145</v>
+        <v>114</v>
       </c>
       <c r="W32">
         <v>1</v>
@@ -2804,34 +2806,34 @@
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B33" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C33">
-        <v>1414</v>
+        <v>1122</v>
       </c>
       <c r="D33">
         <v>2</v>
       </c>
       <c r="E33" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="F33" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="G33" t="s">
+        <v>95</v>
+      </c>
+      <c r="H33" t="s">
+        <v>119</v>
+      </c>
+      <c r="I33" t="s">
         <v>120</v>
       </c>
-      <c r="H33" t="s">
-        <v>151</v>
-      </c>
-      <c r="I33" t="s">
-        <v>152</v>
-      </c>
       <c r="J33" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="L33">
         <v>566</v>
@@ -2858,7 +2860,7 @@
         <v>153</v>
       </c>
       <c r="T33" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="W33">
         <v>1</v>

</xml_diff>